<commit_message>
debugging mac_lane int mode
</commit_message>
<xml_diff>
--- a/npu_v2/diagram/chk_mac_lane.xlsx
+++ b/npu_v2/diagram/chk_mac_lane.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thouh\Desktop\npu\npu_v2\diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E91BCF-260B-42F3-B736-1053285A8125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE2237A-7A82-4F7D-A62A-BDB8814924E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{53E9A3FA-CEF7-4932-8EF3-8B3490928C61}"/>
   </bookViews>
@@ -422,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10ADEE1D-78A8-44C8-96DA-53CE0D481610}">
-  <dimension ref="A1:BM5"/>
+  <dimension ref="A1:BM10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+      <selection activeCell="BK19" sqref="BK19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -628,6 +628,10 @@
       <c r="BL3">
         <v>208</v>
       </c>
+      <c r="BM3">
+        <f t="shared" ref="BM3:BM4" si="0">SUM(A3:BL3)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:65" x14ac:dyDescent="0.45">
       <c r="A4">
@@ -821,6 +825,10 @@
       </c>
       <c r="BL4">
         <v>201</v>
+      </c>
+      <c r="BM4">
+        <f t="shared" si="0"/>
+        <v>-1451</v>
       </c>
     </row>
     <row r="5" spans="1:65" x14ac:dyDescent="0.45">
@@ -829,260 +837,482 @@
         <v>5628</v>
       </c>
       <c r="B5">
-        <f t="shared" ref="B5:BL5" si="0">B3*B4</f>
+        <f t="shared" ref="B5:BL5" si="1">B3*B4</f>
         <v>27000</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-15996</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-33600</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-37828</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4161</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-25098</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-19158</v>
       </c>
       <c r="I5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-23937</v>
       </c>
       <c r="J5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-4800</v>
       </c>
       <c r="K5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36966</v>
       </c>
       <c r="L5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43739</v>
       </c>
       <c r="M5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-15552</v>
       </c>
       <c r="N5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-18360</v>
       </c>
       <c r="O5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-40660</v>
       </c>
       <c r="P5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3402</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-5566</v>
       </c>
       <c r="R5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>57150</v>
       </c>
       <c r="S5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-567</v>
       </c>
       <c r="T5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-12580</v>
       </c>
       <c r="U5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-13662</v>
       </c>
       <c r="V5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-39609</v>
       </c>
       <c r="W5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17556</v>
       </c>
       <c r="X5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9798</v>
       </c>
       <c r="Y5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-22950</v>
       </c>
       <c r="Z5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-28558</v>
       </c>
       <c r="AA5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-8064</v>
       </c>
       <c r="AB5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-10001</v>
       </c>
       <c r="AC5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-32472</v>
       </c>
       <c r="AD5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1098</v>
       </c>
       <c r="AE5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2640</v>
       </c>
       <c r="AF5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-37664</v>
       </c>
       <c r="AG5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-10005</v>
       </c>
       <c r="AH5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-9660</v>
       </c>
       <c r="AI5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13284</v>
       </c>
       <c r="AJ5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1449</v>
       </c>
       <c r="AK5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>57057</v>
       </c>
       <c r="AL5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-5928</v>
       </c>
       <c r="AM5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1485</v>
       </c>
       <c r="AN5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2652</v>
       </c>
       <c r="AO5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>576</v>
       </c>
       <c r="AP5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-26445</v>
       </c>
       <c r="AQ5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2585</v>
       </c>
       <c r="AR5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23217</v>
       </c>
       <c r="AS5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>42720</v>
       </c>
       <c r="AT5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-17220</v>
       </c>
       <c r="AU5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-32832</v>
       </c>
       <c r="AV5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28951</v>
       </c>
       <c r="AW5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17262</v>
       </c>
       <c r="AX5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2640</v>
       </c>
       <c r="AY5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21384</v>
       </c>
       <c r="AZ5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18705</v>
       </c>
       <c r="BA5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21476</v>
       </c>
       <c r="BB5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5112</v>
       </c>
       <c r="BC5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22576</v>
       </c>
       <c r="BD5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16632</v>
       </c>
       <c r="BE5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-7875</v>
       </c>
       <c r="BF5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-8460</v>
       </c>
       <c r="BG5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-51968</v>
       </c>
       <c r="BH5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-33810</v>
       </c>
       <c r="BI5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3616</v>
       </c>
       <c r="BJ5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5104</v>
       </c>
       <c r="BK5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6076</v>
       </c>
       <c r="BL5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41808</v>
       </c>
       <c r="BM5">
         <f>SUM(A5:BL5)</f>
         <v>-101698</v>
+      </c>
+    </row>
+    <row r="6" spans="1:65" x14ac:dyDescent="0.45">
+      <c r="AG6">
+        <v>145</v>
+      </c>
+      <c r="AH6">
+        <v>140</v>
+      </c>
+      <c r="AI6">
+        <v>123</v>
+      </c>
+      <c r="AJ6">
+        <v>-21</v>
+      </c>
+      <c r="AK6">
+        <v>-247</v>
+      </c>
+      <c r="AL6">
+        <v>228</v>
+      </c>
+      <c r="AM6">
+        <v>9</v>
+      </c>
+      <c r="AN6">
+        <v>-221</v>
+      </c>
+      <c r="AO6">
+        <v>192</v>
+      </c>
+      <c r="AP6">
+        <v>123</v>
+      </c>
+      <c r="AQ6">
+        <v>-55</v>
+      </c>
+      <c r="AR6">
+        <v>213</v>
+      </c>
+      <c r="AS6">
+        <v>-178</v>
+      </c>
+      <c r="AT6">
+        <v>-84</v>
+      </c>
+      <c r="AU6">
+        <v>-171</v>
+      </c>
+      <c r="AV6">
+        <v>-131</v>
+      </c>
+      <c r="AW6">
+        <v>-126</v>
+      </c>
+      <c r="AX6">
+        <v>-176</v>
+      </c>
+      <c r="AY6">
+        <v>-198</v>
+      </c>
+      <c r="AZ6">
+        <v>-145</v>
+      </c>
+      <c r="BA6">
+        <v>91</v>
+      </c>
+      <c r="BB6">
+        <v>-24</v>
+      </c>
+      <c r="BC6">
+        <v>-166</v>
+      </c>
+      <c r="BD6">
+        <v>-126</v>
+      </c>
+      <c r="BE6">
+        <v>35</v>
+      </c>
+      <c r="BF6">
+        <v>-47</v>
+      </c>
+      <c r="BG6">
+        <v>203</v>
+      </c>
+      <c r="BH6">
+        <v>147</v>
+      </c>
+      <c r="BI6">
+        <v>-32</v>
+      </c>
+      <c r="BJ6">
+        <v>58</v>
+      </c>
+      <c r="BK6">
+        <v>-217</v>
+      </c>
+      <c r="BL6">
+        <v>208</v>
+      </c>
+      <c r="BM6">
+        <f t="shared" ref="BM6:BM10" si="2">SUM(A6:BL6)</f>
+        <v>-450</v>
+      </c>
+    </row>
+    <row r="7" spans="1:65" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>134</v>
+      </c>
+      <c r="B7">
+        <v>-216</v>
+      </c>
+      <c r="C7">
+        <v>-86</v>
+      </c>
+      <c r="D7">
+        <v>140</v>
+      </c>
+      <c r="E7">
+        <v>196</v>
+      </c>
+      <c r="F7">
+        <v>-73</v>
+      </c>
+      <c r="G7">
+        <v>-141</v>
+      </c>
+      <c r="H7">
+        <v>93</v>
+      </c>
+      <c r="I7">
+        <v>-237</v>
+      </c>
+      <c r="J7">
+        <v>60</v>
+      </c>
+      <c r="K7">
+        <v>183</v>
+      </c>
+      <c r="L7">
+        <v>-229</v>
+      </c>
+      <c r="M7">
+        <v>192</v>
+      </c>
+      <c r="N7">
+        <v>-216</v>
+      </c>
+      <c r="O7">
+        <v>-214</v>
+      </c>
+      <c r="P7">
+        <v>-14</v>
+      </c>
+      <c r="Q7">
+        <v>-23</v>
+      </c>
+      <c r="R7">
+        <v>225</v>
+      </c>
+      <c r="S7">
+        <v>7</v>
+      </c>
+      <c r="T7">
+        <v>148</v>
+      </c>
+      <c r="U7">
+        <v>99</v>
+      </c>
+      <c r="V7">
+        <v>-163</v>
+      </c>
+      <c r="W7">
+        <v>133</v>
+      </c>
+      <c r="X7">
+        <v>138</v>
+      </c>
+      <c r="Y7">
+        <v>-135</v>
+      </c>
+      <c r="Z7">
+        <v>218</v>
+      </c>
+      <c r="AA7">
+        <v>96</v>
+      </c>
+      <c r="AB7">
+        <v>137</v>
+      </c>
+      <c r="AC7">
+        <v>246</v>
+      </c>
+      <c r="AD7">
+        <v>-6</v>
+      </c>
+      <c r="AE7">
+        <v>-20</v>
+      </c>
+      <c r="AF7">
+        <v>-214</v>
+      </c>
+      <c r="BM7">
+        <f t="shared" si="2"/>
+        <v>458</v>
+      </c>
+    </row>
+    <row r="8" spans="1:65" x14ac:dyDescent="0.45">
+      <c r="BM8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:65" x14ac:dyDescent="0.45">
+      <c r="BM9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:65" x14ac:dyDescent="0.45">
+      <c r="BM10">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>